<commit_message>
Finished new guide quests
</commit_message>
<xml_diff>
--- a/resources/data-imports/Quests/guide-quests.xlsx
+++ b/resources/data-imports/Quests/guide-quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="342">
   <si>
     <t>id</t>
   </si>
@@ -38,6 +38,9 @@
     <t>required_level</t>
   </si>
   <si>
+    <t>required_reincarnation_amount</t>
+  </si>
+  <si>
     <t>required_skill</t>
   </si>
   <si>
@@ -179,6 +182,12 @@
     <t>required_fame_level</t>
   </si>
   <si>
+    <t>required_delve_survival_time</t>
+  </si>
+  <si>
+    <t>required_delve_pack_size</t>
+  </si>
+  <si>
     <t>Welcome to Tlessa</t>
   </si>
   <si>
@@ -936,6 +945,102 @@
   </si>
   <si>
     <t>Essence of Rage</t>
+  </si>
+  <si>
+    <t>Unlocking the Delve</t>
+  </si>
+  <si>
+    <t>Its been a long time since you travelled the planes seeking the truth of The Child. Its been a while since yo experienced the thrill of the chase, alas you have become tired with the constant manipulations and slight nudges in a direction that seem s to be out of your control.&lt;br /&gt; &lt;br /&gt; Alas you have finally had enough of the books you pour through searching for something beyond your grasp. As you sit in the old library a voice from the shadows beyond the light of your candle flame dances on the still and quiet air.&lt;br /&gt; &lt;br /&gt; “You wont find what your searching for in those old musty old tomes child.”&lt;br /&gt; &lt;br /&gt; You know the voice, The Guide.&lt;br /&gt; &lt;br /&gt; “You have to go out there and face the harsh realities of the world and to do it, you will need to get a tad bit more stronger.”&lt;br /&gt; &lt;br /&gt; You stare into the void, and you see a hooded figure emerge into the circle of light your candle emits.&lt;br /&gt; &lt;br /&gt; “Remember when you use to face the beasts, hunt the treasure? Seek the answers? Your too busy now with your nose in a book, hunting something beyond your comprehension.”&lt;br /&gt; &lt;br /&gt; Maybe hes right, maybe you do need to refocus your efforts for what might lay ahead.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;By now you would have at least &lt;a href="/information/reincarnation" target="_blank"&gt;reincarnated&lt;/a&gt; once. If not we will need to do it at least ten times. To do this, its very simple:&lt;/p&gt;&lt;p&gt;- Level to level 5,000&lt;/p&gt;&lt;p&gt;- Go to character sheet&lt;/p&gt;&lt;p&gt;- Click reincarnate&lt;/p&gt;&lt;p&gt;- Pay the cost&lt;/p&gt;&lt;p&gt;You will be levelled back to level 1, you will repeat the level up to 5,000 again and then reincarnate again. Exploration is the best for this, as well as Goblin Shop items that give you more XP and double levels&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;All we have to do to reincarnate is:&lt;/p&gt;&lt;p&gt;- Level the character to level 5,000. Exploration is the best way to do this, along with alchemy items from the goblin shop that give you additional levels on level up and additional xp. At this stage you will probably also have quest items that give you bonus xp as well.&lt;/p&gt;&lt;p&gt;- Next, once you are level 5,000 head to Character Sheet tab and click Reincarnate which will be under your currencies on the right hand side.&lt;/p&gt;&lt;p&gt;- Clicking reincarnate will tell you will cost 50,000 copper coins. Paying the price will reset your level back to 1, but you will carry a percentage of your non modified stats over, doing this over and over again will make your character stronger over time.&lt;/p&gt;&lt;p&gt;Repeat these steps until you have reincarnated at least ten times.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;All we have to do to reincarnate is:&lt;/p&gt;&lt;p&gt;- Level the character to level 5,000. Exploration is the best way to do this, along with alchemy items from the goblin shop that give you additional levels on level up and additional xp. At this stage you will probably also have quest items that give you bonus xp as well.&lt;/p&gt;&lt;p&gt;- Next, once you are level 5,000 head to Character Sheet tab and expand the character details section, then click Reincarnate which will be under your currencies..&lt;/p&gt;&lt;p&gt;- Clicking reincarnate will tell you will cost 50,000 copper coins. Paying the price will reset your level back to 1, but you will carry a percentage of your non modified stats over, doing this over and over again will make your character stronger over time.&lt;/p&gt;&lt;p&gt;Repeat these steps until you have reincarnated at least ten times.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The Emerald Mirror</t>
+  </si>
+  <si>
+    <t>Your training has been long, you have been fighting creatures left right and center, you remember the rush, the thrill, the excitement of slaughtering, of finding treasures. You return to the old library one night and flip through some pages, sitting in the silence and the darkness with the only light being a small candle to illuminate the words on the page.&lt;br /&gt; &lt;br /&gt; “You have gotten stronger.” Comes the voice of The Guide.&lt;br /&gt; &lt;br /&gt; You acknowledge this fact.&lt;br /&gt; &lt;br /&gt; “You are ready to search for the answers.”&lt;br /&gt; &lt;br /&gt; You look at his with a quizzical look on your face.&lt;br /&gt; &lt;br /&gt; “You must speak to a mysterious man in the land of memories twisted by delusional thoughts. Find him, search out his request, pull on the thread child.”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We have done quests before, we have done a lot of quests, but to unlock the new mechanic known as Delve, you need to be strong. What we did in the last Guide Quest will only take you so far. Alas now its time to expose the truth of The Child, to expose who The Emerald Prince is, but to do that we have to start on the quest to unlock the secrets of The Emerald Mirror.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We just have to complete a quest, which we have done countless times before.&lt;/p&gt;&lt;p&gt;- Click Quests Tab&lt;/p&gt;&lt;p&gt;- Click Planes, Selected Twisted Memories&lt;/p&gt;&lt;p&gt;- Complete the quest: The Mysterious, Yet Familiar Man&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The Mysterious, Yet Familiar Man</t>
+  </si>
+  <si>
+    <t>The Ever Burning Candle</t>
+  </si>
+  <si>
+    <t>You have started down a long path, one that will answer and deceive you of questions you seek answers to. You are so use to pulling the threads, regardless of consequences, alas now you will be pushed, pushed towards a cave full of shadows, a place where you will delve deep into a new world.&lt;br /&gt; &lt;br /&gt; What will you find in the shadows child? What lies and deceptions, what manipulations will you be forced into? Will it be your own choice? Only one way to find out.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Its time we unlock a new exploration feature called Delve. To do so you will need to complete the quest: A price to pay. A game to win.&lt;/p&gt;&lt;p&gt;Continue following the quest lines until you complete said quest and obtain the Ever Burning Candle. This will unlock the new delve mechanic. Don;t worry child, we will explain more soon!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We just have to complete a quest, which we have done countless times before.&lt;/p&gt;&lt;p&gt;- Click Quests Tab&lt;/p&gt;&lt;p&gt;- Click Planes, Selected Twisted Memories&lt;/p&gt;&lt;p&gt;- Complete the quests until you complete: A price to pay. A Game to win, which will be on Labyrinth.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>A price to play. A game to win</t>
+  </si>
+  <si>
+    <t>Ever Burning Candle</t>
+  </si>
+  <si>
+    <t>Surviving the shadows</t>
+  </si>
+  <si>
+    <t>“I see you have the Ever Burning Candle child.” You turn and see The Guide. You explain how you got it, how everything is becoming a game to these people. You then wonder if The Guide is apart of the same game, ever pushing, ever guiding, ever manipulating.&lt;br /&gt; &lt;br /&gt; “If you are to continue pulling strings child, you’ll need to survive the shadows of your own mind, one that’s growing with paranoia.”&lt;br /&gt; &lt;br /&gt; You look down at the candle, its flame never seems to go out, it never seems to do any damage to any item you place it in. even trying to smother the flame doesn’t work.&lt;br /&gt; &lt;br /&gt; You look at The Guide. You study his face, you see the truth, you have to delve deep into the shadows to keep pushing forward.&lt;br /&gt; &lt;br /&gt; “Take the plunge and survive child. It’s the only way forward.”&lt;br /&gt; &lt;br /&gt; You look back at the candle. Knowing the truth of the matter.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;So far we have completed some quests and reincarnated a bunch of times, but why? Why go through all that?&lt;/p&gt;&lt;p&gt;This all leads to a new feature: Delve.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/delve" target="_blank"&gt;Delve&lt;/a&gt; is a new end game concept that allows you to use a special form of exploration at specific locations that support Delve.&lt;/p&gt;&lt;p&gt;The creatures at these locations are much stronger then any plane, which is why we had you reincarnate so much and then start completing quests to unlock this feature.&lt;/p&gt;&lt;p&gt;The goal of Delve is to survive – the longer the better. The &lt;a href="/information/delve" target="_blank"&gt;info section&lt;/a&gt; has a breakdown of the rewards, alas let me give you something to drool at – last 6+ hours and you get a cosmic item. What fun!&lt;/p&gt;&lt;p&gt;Delve will also be useful because these locations also drop quest items that you will need to progress the story, especially for the next Guide Quest.&lt;/p&gt;&lt;p&gt;Quest items that drop from Delve locations always use your looting skill, to its fullest, so if you have 100% looting chance, the item will auto drop for you.&lt;/p&gt;&lt;p&gt;Delve doesn’t let you select a monster or how long you will fight for, its random monster every fight and the delve goes for 8 hours. You are not meant to, and may not ever – survive all 8 hours. Its about refining your character, your gear, your stats, your class rank abilities, reincarnating to push your self as far as you can go.&lt;/p&gt;&lt;p&gt;Your goal for this Guide Quest is to survive for 1 hour at Cave of Shadows in Twisted Memories.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Now that you have the Ever Burning Candle, make sure you are Twisted Memories and teleport to Cave of Shadows.&lt;/p&gt;&lt;p&gt;Click Exploration and then select the new Delve Mechanic. You cannot manually fight here, nor can you do regular exploration here.&lt;/p&gt;&lt;p&gt;Select your attack type and click Delve.&lt;/p&gt;&lt;p&gt;From here your in a form of exploration. All the Exploration rules will apply.&lt;/p&gt;&lt;p&gt;Now all you have to do is sit back and relax and wait, 1 hour.&lt;/p&gt;&lt;p&gt;You can cancel the delve at any time, if you stay longer then an hour quest items might start dropping.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Now that you have the Ever Burning Candle, make sure you are Twisted Memories and teleport to Cave of Shadows.&lt;/p&gt;&lt;p&gt;Select Exploration from the drop down actions and then select the new Delve Mechanic. You cannot manually fight here, nor can you do regular exploration here.&lt;/p&gt;&lt;p&gt;Select your attack type and click Delve.&lt;/p&gt;&lt;p&gt;From here your in a form of exploration. All the Exploration rules will apply.&lt;/p&gt;&lt;p&gt;Now all you have to do is sit back and relax and wait, 1 hour.&lt;/p&gt;&lt;p&gt;You can cancel the delve at any time, if you stay longer then an hour quest items might start dropping.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Hordes of enemies</t>
+  </si>
+  <si>
+    <t>You managed to crawl from the depths of the shadows with your own treasures and trinkets. You are bruised, bloody and exhausted from your adventures.&lt;br /&gt; &lt;br /&gt; “One on one is no fun child, have you tried groups of enemies? The hordes of the darkness?”&lt;br /&gt; &lt;br /&gt; The Guides voice is laced with laughter at your ability to barley survive the depths of your own twisted mind.&lt;br /&gt; &lt;br /&gt; “The Cave of Shadows is no ones friend child. It is full of the whispers of the past.”&lt;br /&gt; &lt;br /&gt; You stare at The Guide, or more through him as you see the images of the beasts clawing at you from the darkness while you try and survive the depths.&lt;br /&gt; &lt;br /&gt; “Your not done yet child. You have to face the hordes, to do that you will need Clasp of silver dreams. Can you find that child?”&lt;br /&gt; &lt;br /&gt; You regain your senses and agree, but first you must rest. The Guide laughs.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Back to questing child! Now we want to complete quests until we finally reach: &lt;strong&gt;Help me see in the dark&lt;/strong&gt;. This quest will be on &lt;strong&gt;Labyrinth&lt;/strong&gt; and from &lt;strong&gt;The Candle Maker.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Complete this quest and you will get a quest item that then allows you to select a pack size while you set up &lt;a href="/information/delve" target="_blank"&gt;delve&lt;/a&gt;. Pack sizes come with their own benefits for example a pack size of 25 creatures gets you +200% XP bonus which is applied to your total xp, which includes all modifiers, bonuses and so on.&lt;/p&gt;&lt;p&gt;A pack size is exactly that: A pack of creatures you have to fight, one by one. When it comes to the locations enemy strength increase per fight, in this case +3.25% per fight, that modifier is applied to all creatures in that pack. For example: you fight pack A, it has 25 creatures they all have 3.25% increase to their stats. You fight pack B, it has 25 creatures, they all 6.50% increase to their stats, and so on.&lt;/p&gt;&lt;p&gt;Just like monsters, packs are always a new random monster per new round of delve. All packs are made up of the same monster, your packs will never be formed of random monsters.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Once you have the Clasp of silver dreams, head back to Cave of Shadows on twisted Memories and this time select a pack size of at least 5 (you can go higher if you like, but 5 is the minimum). Then select your attack type and begin Delve.&lt;/p&gt;&lt;p&gt;Survive for at least 1 hour.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Help me see in the dark</t>
+  </si>
+  <si>
+    <t>Clasp of silver dreams</t>
+  </si>
+  <si>
+    <t>The Final Test</t>
+  </si>
+  <si>
+    <t>Again you pull yourself from the shadows, bruised and bloody.&lt;br /&gt; &lt;br /&gt; Again you find The Guide, again your pulled in so many directions, manipulated, deceived, lied to. The Child started to play more of a role in trying desperately to keep something hidden, yet everyone else is pushing you towards the inevitable.&lt;br /&gt; &lt;br /&gt; “Having fun?” comes a familiar voice.&lt;br /&gt; &lt;br /&gt; You shake your head, you tell him you wonder how you let things get this far, how you just kept pulling the threads.&lt;br /&gt; &lt;br /&gt; “Curiosity killed the cat you know. Just ask Mr. Whiskers, then again that was more old age … Hmm. Well you get my point child.”&lt;br /&gt; &lt;br /&gt; Is this curiosity or some kind of sick delusional fascination with a broken and warmed mind that is playing a game where the rules constantly change.&lt;br /&gt; &lt;br /&gt; “Such an unhealthy relationship you have managed to entangle your self in. Alas you have to keep going, you have to find the answers, you have to alleviate the curiosity even if it’s just for now.”&lt;br /&gt; &lt;br /&gt; Do you? You ask, Do I really need to keep going?&lt;br /&gt; &lt;br /&gt; “For my own vicarious amusement and morbid curiosity you do. Hahahaha”&lt;br /&gt; &lt;br /&gt; You look at him with a scowl of anger.&lt;br /&gt; &lt;br /&gt; You know he’s right though.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;At this stage, we know how to Delve, how to complete quests and how to reincarnate, so lets finish The Emerald Mirror story line shall we?&lt;/p&gt;&lt;p&gt;All you have to do is complete the story line until you reach and complete: The beating heart at the center.&lt;/p&gt;&lt;p&gt;Then survive in Delve for 2 hours with a pack size that is equal to or greater then 10&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Complete the remaining quests until you reach the end of The Emerald Mirror story line: The beating heart at the center.&lt;/p&gt;&lt;p&gt;Survive a pack size of 10 or greater for 2 or more hours in Delve.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The beating heart at the center</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1380,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BE45"/>
+  <dimension ref="A1:BH51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,59 +1395,62 @@
     <col min="5" max="5" width="2512.672" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="2808.743" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="29.421" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="36.42" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="23.423" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="30.564" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="38.848" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="30.564" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="23.423" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="29.421" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="28.136" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="22.28" bestFit="true" customWidth="true" style="0"/>
-    <col min="24" max="24" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="25" max="25" width="25.851" bestFit="true" customWidth="true" style="0"/>
-    <col min="26" max="26" width="22.28" bestFit="true" customWidth="true" style="0"/>
-    <col min="27" max="27" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="28" max="28" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="35.277" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="24.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="29.421" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="36.42" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="30.564" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="38.848" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="30.564" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="24.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="38.848" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="22.28" bestFit="true" customWidth="true" style="0"/>
+    <col min="25" max="25" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="26" max="26" width="25.851" bestFit="true" customWidth="true" style="0"/>
+    <col min="27" max="27" width="22.28" bestFit="true" customWidth="true" style="0"/>
+    <col min="28" max="28" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="29" max="29" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="34.135" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="37.705" bestFit="true" customWidth="true" style="0"/>
-    <col min="32" max="32" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="30" max="30" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="31" max="31" width="34.135" bestFit="true" customWidth="true" style="0"/>
+    <col min="32" max="32" width="37.705" bestFit="true" customWidth="true" style="0"/>
     <col min="33" max="33" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="35" max="35" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="34" max="34" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="35" max="35" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="36" max="36" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="37" max="37" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="38" max="38" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="39" max="39" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="40" max="40" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="41" max="41" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="42" max="42" width="19.995" bestFit="true" customWidth="true" style="0"/>
-    <col min="43" max="43" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="44" max="44" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="45" max="45" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="46" max="46" width="43.561" bestFit="true" customWidth="true" style="0"/>
-    <col min="47" max="47" width="9.10" bestFit="true" style="0"/>
-    <col min="48" max="48" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="49" max="49" width="9.10" bestFit="true" style="0"/>
-    <col min="50" max="50" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="51" max="51" width="9.10" bestFit="true" style="0"/>
-    <col min="52" max="52" width="23.423" bestFit="true" customWidth="true" style="0"/>
-    <col min="53" max="53" width="39.99" bestFit="true" customWidth="true" style="0"/>
-    <col min="54" max="54" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="55" max="55" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="56" max="56" width="28.136" bestFit="true" customWidth="true" style="0"/>
-    <col min="57" max="57" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="41" max="41" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="42" max="42" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="43" max="43" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="44" max="44" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="45" max="45" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="46" max="46" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="47" max="47" width="43.561" bestFit="true" customWidth="true" style="0"/>
+    <col min="48" max="48" width="9.10" bestFit="true" style="0"/>
+    <col min="49" max="49" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="50" max="50" width="9.10" bestFit="true" style="0"/>
+    <col min="51" max="51" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="52" max="52" width="9.10" bestFit="true" style="0"/>
+    <col min="53" max="53" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="54" max="54" width="39.99" bestFit="true" customWidth="true" style="0"/>
+    <col min="55" max="55" width="24.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="56" max="56" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="57" max="57" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="58" max="58" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="59" max="59" width="34.135" bestFit="true" customWidth="true" style="0"/>
+    <col min="60" max="60" width="29.421" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57">
+    <row r="1" spans="1:60">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1481,13 +1589,13 @@
       <c r="AT1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AU1" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="AY1" t="s">
         <v>48</v>
       </c>
       <c r="BA1" t="s">
@@ -1505,1959 +1613,2214 @@
       <c r="BE1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:57">
+      <c r="BF1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:60">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G2">
         <v>2</v>
       </c>
-      <c r="AR2">
+      <c r="AS2">
         <v>500</v>
       </c>
-      <c r="AS2">
+      <c r="AT2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:57">
+    <row r="3" spans="1:60">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G3">
         <v>10</v>
       </c>
-      <c r="P3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q3">
+      <c r="Q3" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3">
         <v>1</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>500</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:57">
+    <row r="4" spans="1:60">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G4">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4">
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4">
         <v>10</v>
       </c>
-      <c r="J4" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4">
+      <c r="K4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4">
         <v>15</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>50</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>1000</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:57">
+    <row r="5" spans="1:60">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G5">
         <v>50</v>
       </c>
-      <c r="H5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I5">
+      <c r="I5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5">
         <v>5</v>
       </c>
-      <c r="J5" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5">
+      <c r="K5" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5">
         <v>5</v>
       </c>
-      <c r="T5" t="s">
-        <v>79</v>
-      </c>
       <c r="U5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AR5">
+        <v>82</v>
+      </c>
+      <c r="V5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS5">
         <v>1000</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:57">
+    <row r="6" spans="1:60">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G6">
         <v>60</v>
       </c>
-      <c r="H6" t="s">
-        <v>85</v>
-      </c>
-      <c r="I6">
+      <c r="I6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6">
         <v>5</v>
       </c>
-      <c r="J6" t="s">
-        <v>86</v>
-      </c>
-      <c r="K6">
+      <c r="K6" t="s">
+        <v>89</v>
+      </c>
+      <c r="L6">
         <v>15</v>
       </c>
-      <c r="T6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AL6">
+      <c r="U6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM6">
         <v>125</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>10000</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:57">
+    <row r="7" spans="1:60">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G7">
         <v>120</v>
       </c>
-      <c r="H7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I7">
+      <c r="I7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7">
         <v>15</v>
       </c>
-      <c r="J7" t="s">
-        <v>94</v>
-      </c>
-      <c r="K7">
+      <c r="K7" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7">
         <v>5</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>1</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>10</v>
       </c>
-      <c r="T7" t="s">
-        <v>95</v>
-      </c>
-      <c r="W7">
+      <c r="U7" t="s">
+        <v>98</v>
+      </c>
+      <c r="X7">
         <v>500</v>
       </c>
-      <c r="AH7">
+      <c r="AI7">
         <v>210</v>
       </c>
-      <c r="AP7">
+      <c r="AQ7">
         <v>500</v>
       </c>
-      <c r="AQ7">
+      <c r="AR7">
         <v>0</v>
       </c>
-      <c r="AR7">
+      <c r="AS7">
         <v>100000</v>
       </c>
-      <c r="AS7">
+      <c r="AT7">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:57">
+    <row r="8" spans="1:60">
       <c r="A8">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F8" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>67</v>
+      </c>
+      <c r="R8">
+        <v>3</v>
+      </c>
+      <c r="T8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ8">
+        <v>1000</v>
+      </c>
+      <c r="AR8">
         <v>100</v>
       </c>
-      <c r="P8" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q8">
-        <v>3</v>
-      </c>
-      <c r="S8" t="s">
-        <v>101</v>
-      </c>
-      <c r="AP8">
-        <v>1000</v>
-      </c>
-      <c r="AQ8">
+      <c r="AS8">
+        <v>100000</v>
+      </c>
+      <c r="AT8">
         <v>100</v>
       </c>
-      <c r="AR8">
-        <v>100000</v>
-      </c>
-      <c r="AS8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:57">
+    </row>
+    <row r="9" spans="1:60">
       <c r="A9">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I9">
+        <v>108</v>
+      </c>
+      <c r="I9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9">
         <v>50</v>
       </c>
-      <c r="S9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AP9">
+      <c r="T9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ9">
         <v>2500</v>
       </c>
-      <c r="AQ9">
+      <c r="AR9">
         <v>100</v>
       </c>
-      <c r="AR9">
+      <c r="AS9">
         <v>100000</v>
       </c>
-      <c r="AS9">
+      <c r="AT9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:57">
+    <row r="10" spans="1:60">
       <c r="A10">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F10" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G10">
         <v>300</v>
       </c>
-      <c r="P10" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q10">
+      <c r="Q10" t="s">
+        <v>115</v>
+      </c>
+      <c r="R10">
         <v>2</v>
       </c>
-      <c r="R10" t="s">
-        <v>112</v>
-      </c>
-      <c r="T10" t="s">
-        <v>113</v>
-      </c>
-      <c r="AP10">
+      <c r="S10" t="s">
+        <v>115</v>
+      </c>
+      <c r="U10" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ10">
         <v>1000</v>
       </c>
-      <c r="AR10">
+      <c r="AS10">
         <v>500000</v>
       </c>
-      <c r="AS10">
+      <c r="AT10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:57">
+    <row r="11" spans="1:60">
       <c r="A11">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E11" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F11" t="s">
-        <v>118</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
-      <c r="AR11">
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="AS11">
         <v>500000</v>
       </c>
-      <c r="AS11">
+      <c r="AT11">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:57">
+    <row r="12" spans="1:60">
       <c r="A12">
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F12" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA12">
+        <v>126</v>
+      </c>
+      <c r="AB12">
         <v>1</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <v>30</v>
       </c>
-      <c r="AC12">
+      <c r="AD12">
         <v>100</v>
       </c>
-      <c r="AR12">
+      <c r="AS12">
         <v>1000000</v>
       </c>
-      <c r="AS12">
+      <c r="AT12">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:57">
+    <row r="13" spans="1:60">
       <c r="A13">
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E13" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
-        <v>128</v>
-      </c>
-      <c r="H13" t="s">
-        <v>93</v>
-      </c>
-      <c r="I13">
+        <v>131</v>
+      </c>
+      <c r="I13" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13">
         <v>25</v>
       </c>
-      <c r="J13" t="s">
-        <v>129</v>
-      </c>
-      <c r="K13">
+      <c r="K13" t="s">
+        <v>132</v>
+      </c>
+      <c r="L13">
         <v>5</v>
       </c>
-      <c r="AB13">
+      <c r="AC13">
         <v>60</v>
       </c>
-      <c r="AC13">
+      <c r="AD13">
         <v>500</v>
       </c>
-      <c r="AF13" t="s">
-        <v>130</v>
-      </c>
-      <c r="AG13">
+      <c r="AG13" t="s">
+        <v>133</v>
+      </c>
+      <c r="AH13">
         <v>1</v>
       </c>
-      <c r="AR13">
+      <c r="AS13">
         <v>2000000</v>
       </c>
-      <c r="AS13">
+      <c r="AT13">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:57">
+    <row r="14" spans="1:60">
       <c r="A14">
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E14" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F14" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB14">
+        <v>137</v>
+      </c>
+      <c r="AC14">
         <v>75</v>
       </c>
-      <c r="AC14">
+      <c r="AD14">
         <v>2000</v>
       </c>
-      <c r="AF14" t="s">
-        <v>135</v>
-      </c>
-      <c r="AG14">
+      <c r="AG14" t="s">
+        <v>138</v>
+      </c>
+      <c r="AH14">
         <v>2</v>
       </c>
-      <c r="AR14">
+      <c r="AS14">
         <v>2000000</v>
       </c>
-      <c r="AS14">
+      <c r="AT14">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:57">
+    <row r="15" spans="1:60">
       <c r="A15">
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E15" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F15" t="s">
-        <v>139</v>
-      </c>
-      <c r="H15" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15">
+        <v>142</v>
+      </c>
+      <c r="I15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15">
         <v>25</v>
       </c>
-      <c r="J15" t="s">
-        <v>93</v>
-      </c>
-      <c r="K15">
+      <c r="K15" t="s">
+        <v>96</v>
+      </c>
+      <c r="L15">
         <v>50</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>2</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>10</v>
       </c>
-      <c r="S15" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB15">
+      <c r="T15" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC15">
         <v>100</v>
       </c>
-      <c r="AC15">
+      <c r="AD15">
         <v>3000</v>
       </c>
-      <c r="AF15" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG15">
+      <c r="AG15" t="s">
+        <v>144</v>
+      </c>
+      <c r="AH15">
         <v>1</v>
       </c>
-      <c r="AR15">
+      <c r="AS15">
         <v>5000000</v>
       </c>
-      <c r="AS15">
+      <c r="AT15">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:57">
+    <row r="16" spans="1:60">
       <c r="A16">
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E16" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F16" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G16">
         <v>500</v>
       </c>
-      <c r="H16" t="s">
-        <v>93</v>
-      </c>
-      <c r="I16">
+      <c r="I16" t="s">
+        <v>96</v>
+      </c>
+      <c r="J16">
         <v>100</v>
       </c>
-      <c r="J16" t="s">
-        <v>94</v>
-      </c>
-      <c r="K16">
+      <c r="K16" t="s">
+        <v>97</v>
+      </c>
+      <c r="L16">
         <v>50</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>1</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>100</v>
       </c>
-      <c r="P16" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q16">
+      <c r="Q16" t="s">
+        <v>149</v>
+      </c>
+      <c r="R16">
         <v>3</v>
       </c>
-      <c r="R16" t="s">
-        <v>146</v>
-      </c>
       <c r="S16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="T16" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="U16" t="s">
-        <v>149</v>
-      </c>
-      <c r="W16">
+        <v>151</v>
+      </c>
+      <c r="V16" t="s">
+        <v>152</v>
+      </c>
+      <c r="X16">
         <v>25000</v>
       </c>
-      <c r="AQ16">
+      <c r="AR16">
         <v>1000</v>
       </c>
-      <c r="AR16">
+      <c r="AS16">
         <v>50000000</v>
       </c>
-      <c r="AS16">
+      <c r="AT16">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:57">
+    <row r="17" spans="1:60">
       <c r="A17">
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C17" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D17" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E17" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F17" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G17">
         <v>600</v>
       </c>
-      <c r="H17" t="s">
-        <v>155</v>
-      </c>
-      <c r="I17">
+      <c r="I17" t="s">
+        <v>158</v>
+      </c>
+      <c r="J17">
         <v>3</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>3</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>10</v>
       </c>
-      <c r="AP17">
+      <c r="AQ17">
         <v>25000</v>
       </c>
-      <c r="AQ17">
+      <c r="AR17">
         <v>1000</v>
       </c>
-      <c r="AR17">
+      <c r="AS17">
         <v>75000000</v>
       </c>
-      <c r="AS17">
+      <c r="AT17">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:57">
+    <row r="18" spans="1:60">
       <c r="A18">
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D18" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E18" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F18" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G18">
         <v>1000</v>
       </c>
-      <c r="J18" t="s">
-        <v>93</v>
-      </c>
-      <c r="K18">
+      <c r="K18" t="s">
+        <v>96</v>
+      </c>
+      <c r="L18">
         <v>400</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>1</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>400</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>3</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>30</v>
       </c>
-      <c r="S18" t="s">
-        <v>160</v>
-      </c>
-      <c r="AH18">
+      <c r="T18" t="s">
+        <v>163</v>
+      </c>
+      <c r="AI18">
         <v>6000</v>
       </c>
-      <c r="AP18">
+      <c r="AQ18">
         <v>50000</v>
       </c>
-      <c r="AQ18">
+      <c r="AR18">
         <v>5000</v>
       </c>
-      <c r="AR18">
+      <c r="AS18">
         <v>2000000000</v>
       </c>
-      <c r="AS18">
+      <c r="AT18">
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:57">
+    <row r="19" spans="1:60">
       <c r="A19">
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C19" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D19" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G19">
         <v>1500</v>
       </c>
-      <c r="P19" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q19">
+      <c r="Q19" t="s">
+        <v>168</v>
+      </c>
+      <c r="R19">
         <v>2</v>
       </c>
-      <c r="R19" t="s">
-        <v>165</v>
-      </c>
-      <c r="T19" t="s">
-        <v>166</v>
-      </c>
-      <c r="AH19">
+      <c r="S19" t="s">
+        <v>168</v>
+      </c>
+      <c r="U19" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI19">
         <v>7000</v>
       </c>
-      <c r="AR19">
+      <c r="AS19">
         <v>2000000000</v>
       </c>
-      <c r="AS19">
+      <c r="AT19">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:57">
+    <row r="20" spans="1:60">
       <c r="A20">
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D20" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E20" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F20" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G20">
         <v>2000</v>
       </c>
-      <c r="S20" t="s">
-        <v>171</v>
-      </c>
-      <c r="AR20">
+      <c r="T20" t="s">
+        <v>174</v>
+      </c>
+      <c r="AS20">
         <v>2000000000</v>
       </c>
-      <c r="AS20">
+      <c r="AT20">
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:57">
+    <row r="21" spans="1:60">
       <c r="A21">
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C21" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D21" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E21" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F21" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G21">
         <v>2500</v>
       </c>
-      <c r="H21" t="s">
-        <v>155</v>
-      </c>
-      <c r="I21">
+      <c r="I21" t="s">
+        <v>158</v>
+      </c>
+      <c r="J21">
         <v>50</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>13</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>50</v>
       </c>
-      <c r="P21" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q21">
+      <c r="Q21" t="s">
+        <v>168</v>
+      </c>
+      <c r="R21">
         <v>5</v>
       </c>
-      <c r="Z21">
+      <c r="AA21">
         <v>100</v>
       </c>
-      <c r="AA21">
+      <c r="AB21">
         <v>2</v>
       </c>
-      <c r="AC21">
+      <c r="AD21">
         <v>20000</v>
       </c>
-      <c r="AD21" t="s">
-        <v>141</v>
-      </c>
-      <c r="AE21">
+      <c r="AE21" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF21">
         <v>5</v>
       </c>
-      <c r="AP21">
+      <c r="AQ21">
         <v>20000</v>
       </c>
-      <c r="AQ21">
+      <c r="AR21">
         <v>2000</v>
       </c>
-      <c r="AR21">
+      <c r="AS21">
         <v>5000000000</v>
       </c>
-      <c r="AS21">
+      <c r="AT21">
         <v>1500</v>
       </c>
     </row>
-    <row r="22" spans="1:57">
+    <row r="22" spans="1:60">
       <c r="A22">
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C22" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E22" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F22" t="s">
-        <v>180</v>
-      </c>
-      <c r="AR22">
+        <v>183</v>
+      </c>
+      <c r="AS22">
         <v>100000</v>
       </c>
-      <c r="AS22">
+      <c r="AT22">
         <v>50</v>
       </c>
-      <c r="AV22">
+      <c r="AW22">
         <v>25</v>
       </c>
-      <c r="AX22">
+      <c r="AY22">
         <v>3</v>
       </c>
-      <c r="AZ22" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="23" spans="1:57">
+      <c r="BA22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:60">
       <c r="A23">
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C23" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D23" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E23" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F23" t="s">
-        <v>186</v>
-      </c>
-      <c r="AR23">
+        <v>189</v>
+      </c>
+      <c r="AS23">
         <v>100000</v>
       </c>
-      <c r="AS23">
+      <c r="AT23">
         <v>75</v>
       </c>
-      <c r="AT23" t="s">
-        <v>176</v>
-      </c>
-      <c r="AV23">
+      <c r="AU23" t="s">
+        <v>179</v>
+      </c>
+      <c r="AW23">
         <v>25</v>
       </c>
-      <c r="AX23">
+      <c r="AY23">
         <v>3</v>
       </c>
-      <c r="BA23">
+      <c r="BB23">
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:57">
+    <row r="24" spans="1:60">
       <c r="A24">
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C24" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E24" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F24" t="s">
-        <v>190</v>
-      </c>
-      <c r="S24" t="s">
-        <v>191</v>
-      </c>
-      <c r="AP24">
-        <v>5000</v>
+        <v>193</v>
+      </c>
+      <c r="T24" t="s">
+        <v>194</v>
       </c>
       <c r="AQ24">
         <v>5000</v>
       </c>
       <c r="AR24">
+        <v>5000</v>
+      </c>
+      <c r="AS24">
         <v>100000</v>
       </c>
-      <c r="AS24">
+      <c r="AT24">
         <v>100</v>
       </c>
-      <c r="AT24" t="s">
-        <v>176</v>
-      </c>
-      <c r="AV24">
+      <c r="AU24" t="s">
+        <v>179</v>
+      </c>
+      <c r="AW24">
         <v>25</v>
       </c>
-      <c r="AX24">
+      <c r="AY24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:57">
+    <row r="25" spans="1:60">
       <c r="A25">
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C25" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D25" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E25" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F25" t="s">
-        <v>195</v>
-      </c>
-      <c r="S25" t="s">
-        <v>196</v>
-      </c>
-      <c r="AP25">
-        <v>1000</v>
+        <v>198</v>
+      </c>
+      <c r="T25" t="s">
+        <v>199</v>
       </c>
       <c r="AQ25">
         <v>1000</v>
       </c>
       <c r="AR25">
+        <v>1000</v>
+      </c>
+      <c r="AS25">
         <v>500000</v>
       </c>
-      <c r="AS25">
+      <c r="AT25">
         <v>100</v>
       </c>
-      <c r="AT25" t="s">
-        <v>187</v>
-      </c>
-      <c r="AV25">
+      <c r="AU25" t="s">
+        <v>190</v>
+      </c>
+      <c r="AW25">
         <v>25</v>
       </c>
-      <c r="AX25">
+      <c r="AY25">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:57">
+    <row r="26" spans="1:60">
       <c r="A26">
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C26" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D26" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E26" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F26" t="s">
-        <v>200</v>
-      </c>
-      <c r="S26" t="s">
-        <v>201</v>
-      </c>
-      <c r="AP26">
-        <v>2000</v>
+        <v>203</v>
+      </c>
+      <c r="T26" t="s">
+        <v>204</v>
       </c>
       <c r="AQ26">
         <v>2000</v>
       </c>
       <c r="AR26">
+        <v>2000</v>
+      </c>
+      <c r="AS26">
         <v>500000</v>
       </c>
-      <c r="AS26">
+      <c r="AT26">
         <v>100</v>
       </c>
-      <c r="AT26" t="s">
-        <v>176</v>
-      </c>
-      <c r="AV26">
+      <c r="AU26" t="s">
+        <v>179</v>
+      </c>
+      <c r="AW26">
         <v>25</v>
       </c>
-      <c r="AX26">
+      <c r="AY26">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:57">
+    <row r="27" spans="1:60">
       <c r="A27">
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C27" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D27" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E27" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F27" t="s">
-        <v>206</v>
-      </c>
-      <c r="S27" t="s">
-        <v>207</v>
-      </c>
-      <c r="AA27">
+        <v>209</v>
+      </c>
+      <c r="T27" t="s">
+        <v>210</v>
+      </c>
+      <c r="AB27">
         <v>1</v>
       </c>
-      <c r="AB27">
+      <c r="AC27">
         <v>30</v>
       </c>
-      <c r="AC27">
+      <c r="AD27">
         <v>500</v>
       </c>
-      <c r="AF27" t="s">
-        <v>130</v>
-      </c>
-      <c r="AG27">
+      <c r="AG27" t="s">
+        <v>133</v>
+      </c>
+      <c r="AH27">
         <v>1</v>
-      </c>
-      <c r="AP27">
-        <v>1000</v>
       </c>
       <c r="AQ27">
         <v>1000</v>
       </c>
       <c r="AR27">
+        <v>1000</v>
+      </c>
+      <c r="AS27">
         <v>1000000</v>
       </c>
-      <c r="AS27">
+      <c r="AT27">
         <v>100</v>
       </c>
-      <c r="AT27" t="s">
-        <v>176</v>
-      </c>
-      <c r="AV27">
+      <c r="AU27" t="s">
+        <v>179</v>
+      </c>
+      <c r="AW27">
         <v>25</v>
       </c>
-      <c r="AX27">
+      <c r="AY27">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:57">
+    <row r="28" spans="1:60">
       <c r="A28">
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C28" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D28" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E28" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F28" t="s">
-        <v>211</v>
-      </c>
-      <c r="R28" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="S28" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="T28" t="s">
-        <v>214</v>
-      </c>
-      <c r="AP28">
+        <v>216</v>
+      </c>
+      <c r="U28" t="s">
+        <v>217</v>
+      </c>
+      <c r="AQ28">
         <v>25000</v>
       </c>
-      <c r="AQ28">
+      <c r="AR28">
         <v>3000</v>
       </c>
-      <c r="AR28">
+      <c r="AS28">
         <v>8000000000</v>
       </c>
-      <c r="AS28">
+      <c r="AT28">
         <v>2000</v>
       </c>
-      <c r="AZ28" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="29" spans="1:57">
+      <c r="BA28" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:60">
       <c r="A29">
         <v>34</v>
       </c>
       <c r="B29" t="s">
+        <v>218</v>
+      </c>
+      <c r="C29" t="s">
+        <v>219</v>
+      </c>
+      <c r="D29" t="s">
+        <v>220</v>
+      </c>
+      <c r="E29" t="s">
+        <v>221</v>
+      </c>
+      <c r="F29" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q29" t="s">
         <v>215</v>
       </c>
-      <c r="C29" t="s">
-        <v>216</v>
-      </c>
-      <c r="D29" t="s">
-        <v>217</v>
-      </c>
-      <c r="E29" t="s">
-        <v>218</v>
-      </c>
-      <c r="F29" t="s">
-        <v>219</v>
-      </c>
-      <c r="P29" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q29">
+      <c r="R29">
         <v>2</v>
       </c>
-      <c r="AP29">
+      <c r="AQ29">
         <v>25000</v>
       </c>
-      <c r="AQ29">
+      <c r="AR29">
         <v>3000</v>
       </c>
-      <c r="AR29">
+      <c r="AS29">
         <v>8000000000</v>
       </c>
-      <c r="AS29">
+      <c r="AT29">
         <v>2000</v>
       </c>
-      <c r="BD29" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="30" spans="1:57">
+      <c r="BE29" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:60">
       <c r="A30">
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C30" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D30" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F30" t="s">
-        <v>225</v>
-      </c>
-      <c r="P30" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q30">
+        <v>228</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>215</v>
+      </c>
+      <c r="R30">
         <v>5</v>
       </c>
-      <c r="AP30">
+      <c r="AQ30">
         <v>25000</v>
       </c>
-      <c r="AQ30">
+      <c r="AR30">
         <v>3000</v>
       </c>
-      <c r="AR30">
+      <c r="AS30">
         <v>8000000000</v>
       </c>
-      <c r="AS30">
+      <c r="AT30">
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="1:57">
+    <row r="31" spans="1:60">
       <c r="A31">
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C31" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E31" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F31" t="s">
-        <v>229</v>
-      </c>
-      <c r="R31" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="S31" t="s">
-        <v>231</v>
-      </c>
-      <c r="AP31">
+        <v>233</v>
+      </c>
+      <c r="T31" t="s">
+        <v>234</v>
+      </c>
+      <c r="AQ31">
         <v>25000</v>
       </c>
-      <c r="AQ31">
+      <c r="AR31">
         <v>3000</v>
       </c>
-      <c r="AR31">
+      <c r="AS31">
         <v>8000000000</v>
       </c>
-      <c r="AS31">
+      <c r="AT31">
         <v>2000</v>
       </c>
-      <c r="AZ31" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="32" spans="1:57">
+      <c r="BA31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32" spans="1:60">
       <c r="A32">
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C32" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D32" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E32" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F32" t="s">
-        <v>235</v>
-      </c>
-      <c r="H32" t="s">
-        <v>155</v>
-      </c>
-      <c r="I32">
+        <v>238</v>
+      </c>
+      <c r="I32" t="s">
+        <v>158</v>
+      </c>
+      <c r="J32">
         <v>200</v>
       </c>
-      <c r="AP32">
+      <c r="AQ32">
         <v>25000</v>
       </c>
-      <c r="AQ32">
+      <c r="AR32">
         <v>3000</v>
       </c>
-      <c r="AR32">
+      <c r="AS32">
         <v>8000000000</v>
       </c>
-      <c r="AS32">
+      <c r="AT32">
         <v>2000</v>
       </c>
     </row>
-    <row r="33" spans="1:57">
+    <row r="33" spans="1:60">
       <c r="A33">
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C33" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D33" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E33" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F33" t="s">
-        <v>240</v>
-      </c>
-      <c r="S33" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y33">
+        <v>243</v>
+      </c>
+      <c r="T33" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z33">
         <v>5000</v>
       </c>
-      <c r="AP33">
+      <c r="AQ33">
         <v>50000</v>
       </c>
-      <c r="AQ33">
+      <c r="AR33">
         <v>6000</v>
       </c>
-      <c r="AR33">
+      <c r="AS33">
         <v>12000000000</v>
       </c>
-      <c r="AS33">
+      <c r="AT33">
         <v>5000</v>
       </c>
-      <c r="BB33">
+      <c r="BC33">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:57">
+    <row r="34" spans="1:60">
       <c r="A34">
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C34" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D34" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E34" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F34" t="s">
-        <v>245</v>
-      </c>
-      <c r="AP34">
+        <v>248</v>
+      </c>
+      <c r="AQ34">
         <v>50000</v>
       </c>
-      <c r="AQ34">
+      <c r="AR34">
         <v>6000</v>
       </c>
-      <c r="AR34">
+      <c r="AS34">
         <v>12000000000</v>
       </c>
-      <c r="AS34">
+      <c r="AT34">
         <v>5000</v>
       </c>
-      <c r="BD34" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="35" spans="1:57">
+      <c r="BE34" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:60">
       <c r="A35">
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C35" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D35" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E35" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F35" t="s">
-        <v>251</v>
-      </c>
-      <c r="H35" t="s">
-        <v>252</v>
-      </c>
-      <c r="I35">
+        <v>254</v>
+      </c>
+      <c r="I35" t="s">
+        <v>255</v>
+      </c>
+      <c r="J35">
         <v>25</v>
       </c>
-      <c r="AP35">
+      <c r="AQ35">
         <v>100000</v>
       </c>
-      <c r="AQ35">
+      <c r="AR35">
         <v>12000</v>
       </c>
-      <c r="AR35">
+      <c r="AS35">
         <v>16000000000</v>
       </c>
-      <c r="AS35">
+      <c r="AT35">
         <v>8000</v>
       </c>
     </row>
-    <row r="36" spans="1:57">
+    <row r="36" spans="1:60">
       <c r="A36">
         <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C36" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D36" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E36" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F36" t="s">
-        <v>257</v>
-      </c>
-      <c r="P36" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q36">
+        <v>260</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>67</v>
+      </c>
+      <c r="R36">
         <v>5</v>
       </c>
-      <c r="AP36">
+      <c r="AQ36">
         <v>500</v>
       </c>
-      <c r="AQ36">
+      <c r="AR36">
         <v>250</v>
       </c>
-      <c r="AR36">
+      <c r="AS36">
         <v>100000</v>
       </c>
-      <c r="AS36">
+      <c r="AT36">
         <v>100</v>
       </c>
-      <c r="AV36">
+      <c r="AW36">
         <v>1500</v>
       </c>
-      <c r="BE36">
+      <c r="BF36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:57">
+    <row r="37" spans="1:60">
       <c r="A37">
         <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C37" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D37" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E37" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F37" t="s">
-        <v>261</v>
-      </c>
-      <c r="H37" t="s">
-        <v>252</v>
-      </c>
-      <c r="I37">
+        <v>264</v>
+      </c>
+      <c r="I37" t="s">
+        <v>255</v>
+      </c>
+      <c r="J37">
         <v>75</v>
       </c>
-      <c r="S37" t="s">
-        <v>262</v>
-      </c>
-      <c r="AP37">
+      <c r="T37" t="s">
+        <v>265</v>
+      </c>
+      <c r="AQ37">
         <v>150000</v>
       </c>
-      <c r="AQ37">
+      <c r="AR37">
         <v>30000</v>
       </c>
-      <c r="AR37">
+      <c r="AS37">
         <v>32000000000</v>
       </c>
-      <c r="AS37">
+      <c r="AT37">
         <v>8000</v>
       </c>
     </row>
-    <row r="38" spans="1:57">
+    <row r="38" spans="1:60">
       <c r="A38">
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C38" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D38" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="E38" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F38" t="s">
-        <v>267</v>
-      </c>
-      <c r="H38" t="s">
-        <v>252</v>
-      </c>
-      <c r="I38">
+        <v>270</v>
+      </c>
+      <c r="I38" t="s">
+        <v>255</v>
+      </c>
+      <c r="J38">
         <v>150</v>
       </c>
-      <c r="N38">
+      <c r="O38">
         <v>3</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <v>100</v>
       </c>
-      <c r="Z38">
+      <c r="AA38">
         <v>10000</v>
       </c>
-      <c r="AA38">
+      <c r="AB38">
         <v>10</v>
       </c>
-      <c r="AC38">
+      <c r="AD38">
         <v>50000</v>
       </c>
-      <c r="AD38" t="s">
-        <v>268</v>
-      </c>
-      <c r="AE38">
+      <c r="AE38" t="s">
+        <v>271</v>
+      </c>
+      <c r="AF38">
         <v>30</v>
       </c>
-      <c r="AF38" t="s">
-        <v>269</v>
-      </c>
-      <c r="AG38">
+      <c r="AG38" t="s">
+        <v>272</v>
+      </c>
+      <c r="AH38">
         <v>4</v>
       </c>
-      <c r="AP38">
+      <c r="AQ38">
         <v>150000</v>
       </c>
-      <c r="AQ38">
+      <c r="AR38">
         <v>30000</v>
       </c>
-      <c r="AR38">
+      <c r="AS38">
         <v>32000000000</v>
       </c>
-      <c r="AS38">
+      <c r="AT38">
         <v>8000</v>
       </c>
     </row>
-    <row r="39" spans="1:57">
+    <row r="39" spans="1:60">
       <c r="A39">
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C39" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D39" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="E39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="F39" t="s">
-        <v>273</v>
-      </c>
-      <c r="H39" t="s">
-        <v>252</v>
-      </c>
-      <c r="I39">
+        <v>276</v>
+      </c>
+      <c r="I39" t="s">
+        <v>255</v>
+      </c>
+      <c r="J39">
         <v>300</v>
       </c>
-      <c r="AH39">
+      <c r="AI39">
         <v>1000000</v>
       </c>
-      <c r="AP39">
+      <c r="AQ39">
         <v>150000</v>
       </c>
-      <c r="AQ39">
+      <c r="AR39">
         <v>30000</v>
       </c>
-      <c r="AR39">
+      <c r="AS39">
         <v>32000000000</v>
       </c>
-      <c r="AS39">
+      <c r="AT39">
         <v>8000</v>
       </c>
     </row>
-    <row r="40" spans="1:57">
+    <row r="40" spans="1:60">
       <c r="A40">
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C40" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D40" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="E40" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F40" t="s">
-        <v>277</v>
-      </c>
-      <c r="H40" t="s">
-        <v>252</v>
-      </c>
-      <c r="I40">
+        <v>280</v>
+      </c>
+      <c r="I40" t="s">
+        <v>255</v>
+      </c>
+      <c r="J40">
         <v>400</v>
       </c>
-      <c r="S40" t="s">
-        <v>278</v>
-      </c>
       <c r="T40" t="s">
-        <v>279</v>
-      </c>
-      <c r="AH40">
+        <v>281</v>
+      </c>
+      <c r="U40" t="s">
+        <v>282</v>
+      </c>
+      <c r="AI40">
         <v>2000000</v>
       </c>
-      <c r="AP40">
+      <c r="AQ40">
         <v>150000</v>
       </c>
-      <c r="AQ40">
+      <c r="AR40">
         <v>30000</v>
       </c>
-      <c r="AR40">
+      <c r="AS40">
         <v>32000000000</v>
       </c>
-      <c r="AS40">
+      <c r="AT40">
         <v>8000</v>
       </c>
     </row>
-    <row r="41" spans="1:57">
+    <row r="41" spans="1:60">
       <c r="A41">
         <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C41" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D41" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E41" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F41" t="s">
-        <v>283</v>
-      </c>
-      <c r="AH41">
+        <v>286</v>
+      </c>
+      <c r="AI41">
         <v>2500000</v>
       </c>
-      <c r="AP41">
+      <c r="AQ41">
         <v>150000</v>
       </c>
-      <c r="AQ41">
+      <c r="AR41">
         <v>30000</v>
       </c>
-      <c r="AR41">
+      <c r="AS41">
         <v>32000000000</v>
       </c>
-      <c r="AS41">
+      <c r="AT41">
         <v>8000</v>
       </c>
-      <c r="AZ41" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="42" spans="1:57">
+      <c r="BA41" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:60">
       <c r="A42">
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C42" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D42" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E42" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F42" t="s">
-        <v>289</v>
-      </c>
-      <c r="AP42">
-        <v>100</v>
+        <v>292</v>
       </c>
       <c r="AQ42">
         <v>100</v>
       </c>
       <c r="AR42">
+        <v>100</v>
+      </c>
+      <c r="AS42">
         <v>1000</v>
       </c>
-      <c r="AS42">
+      <c r="AT42">
         <v>100</v>
       </c>
-      <c r="AV42">
+      <c r="AW42">
         <v>10</v>
       </c>
-      <c r="AX42">
+      <c r="AY42">
         <v>7</v>
       </c>
-      <c r="AZ42" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="43" spans="1:57">
+      <c r="BA42" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="43" spans="1:60">
       <c r="A43">
         <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C43" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D43" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="E43" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="F43" t="s">
-        <v>295</v>
-      </c>
-      <c r="AP43">
-        <v>100</v>
+        <v>298</v>
       </c>
       <c r="AQ43">
         <v>100</v>
       </c>
       <c r="AR43">
+        <v>100</v>
+      </c>
+      <c r="AS43">
         <v>1000</v>
       </c>
-      <c r="AS43">
+      <c r="AT43">
         <v>100</v>
       </c>
-      <c r="AT43" t="s">
-        <v>285</v>
-      </c>
-      <c r="AX43">
+      <c r="AU43" t="s">
+        <v>288</v>
+      </c>
+      <c r="AY43">
         <v>7</v>
       </c>
-      <c r="AZ43" t="s">
-        <v>290</v>
-      </c>
-      <c r="BA43">
+      <c r="BA43" t="s">
+        <v>293</v>
+      </c>
+      <c r="BB43">
         <v>1000</v>
       </c>
     </row>
-    <row r="44" spans="1:57">
+    <row r="44" spans="1:60">
       <c r="A44">
         <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C44" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D44" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E44" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="F44" t="s">
-        <v>300</v>
-      </c>
-      <c r="S44" t="s">
-        <v>301</v>
-      </c>
-      <c r="AP44">
-        <v>100</v>
+        <v>303</v>
+      </c>
+      <c r="T44" t="s">
+        <v>304</v>
       </c>
       <c r="AQ44">
         <v>100</v>
       </c>
       <c r="AR44">
+        <v>100</v>
+      </c>
+      <c r="AS44">
         <v>1000</v>
       </c>
-      <c r="AS44">
+      <c r="AT44">
         <v>100</v>
       </c>
-      <c r="AT44" t="s">
-        <v>291</v>
-      </c>
-      <c r="AX44">
+      <c r="AU44" t="s">
+        <v>294</v>
+      </c>
+      <c r="AY44">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:57">
+    <row r="45" spans="1:60">
       <c r="A45">
         <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C45" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="D45" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="E45" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="F45" t="s">
-        <v>305</v>
-      </c>
-      <c r="S45" t="s">
-        <v>101</v>
+        <v>308</v>
       </c>
       <c r="T45" t="s">
-        <v>306</v>
-      </c>
-      <c r="AP45">
-        <v>100</v>
+        <v>104</v>
+      </c>
+      <c r="U45" t="s">
+        <v>309</v>
       </c>
       <c r="AQ45">
         <v>100</v>
       </c>
       <c r="AR45">
+        <v>100</v>
+      </c>
+      <c r="AS45">
         <v>1000</v>
       </c>
-      <c r="AS45">
+      <c r="AT45">
         <v>100</v>
       </c>
-      <c r="AT45" t="s">
-        <v>296</v>
-      </c>
-      <c r="AX45">
+      <c r="AU45" t="s">
+        <v>299</v>
+      </c>
+      <c r="AY45">
         <v>7</v>
       </c>
-      <c r="AZ45" t="s">
-        <v>290</v>
+      <c r="BA45" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="46" spans="1:60">
+      <c r="A46">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>310</v>
+      </c>
+      <c r="C46" t="s">
+        <v>311</v>
+      </c>
+      <c r="D46" t="s">
+        <v>312</v>
+      </c>
+      <c r="E46" t="s">
+        <v>313</v>
+      </c>
+      <c r="F46" t="s">
+        <v>314</v>
+      </c>
+      <c r="H46">
+        <v>10</v>
+      </c>
+      <c r="AQ46">
+        <v>50000</v>
+      </c>
+      <c r="AR46">
+        <v>5000</v>
+      </c>
+      <c r="AS46">
+        <v>50000000</v>
+      </c>
+      <c r="AT46">
+        <v>2500</v>
+      </c>
+      <c r="AU46" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="47" spans="1:60">
+      <c r="A47">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>315</v>
+      </c>
+      <c r="C47" t="s">
+        <v>316</v>
+      </c>
+      <c r="D47" t="s">
+        <v>317</v>
+      </c>
+      <c r="E47" t="s">
+        <v>318</v>
+      </c>
+      <c r="F47" t="s">
+        <v>318</v>
+      </c>
+      <c r="S47" t="s">
+        <v>287</v>
+      </c>
+      <c r="T47" t="s">
+        <v>319</v>
+      </c>
+      <c r="AQ47">
+        <v>100000</v>
+      </c>
+      <c r="AR47">
+        <v>10000</v>
+      </c>
+      <c r="AS47">
+        <v>200000000</v>
+      </c>
+      <c r="AT47">
+        <v>10000</v>
+      </c>
+      <c r="AU47" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="48" spans="1:60">
+      <c r="A48">
+        <v>53</v>
+      </c>
+      <c r="B48" t="s">
+        <v>320</v>
+      </c>
+      <c r="C48" t="s">
+        <v>321</v>
+      </c>
+      <c r="D48" t="s">
+        <v>322</v>
+      </c>
+      <c r="E48" t="s">
+        <v>323</v>
+      </c>
+      <c r="F48" t="s">
+        <v>323</v>
+      </c>
+      <c r="T48" t="s">
+        <v>324</v>
+      </c>
+      <c r="U48" t="s">
+        <v>325</v>
+      </c>
+      <c r="AQ48">
+        <v>10000</v>
+      </c>
+      <c r="AR48">
+        <v>10000</v>
+      </c>
+      <c r="AS48">
+        <v>10000000</v>
+      </c>
+      <c r="AT48">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:60">
+      <c r="A49">
+        <v>54</v>
+      </c>
+      <c r="B49" t="s">
+        <v>326</v>
+      </c>
+      <c r="C49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D49" t="s">
+        <v>328</v>
+      </c>
+      <c r="E49" t="s">
+        <v>329</v>
+      </c>
+      <c r="F49" t="s">
+        <v>330</v>
+      </c>
+      <c r="AQ49">
+        <v>100000</v>
+      </c>
+      <c r="AR49">
+        <v>100000</v>
+      </c>
+      <c r="AS49">
+        <v>1000000000</v>
+      </c>
+      <c r="AT49">
+        <v>25000</v>
+      </c>
+      <c r="AU49" t="s">
+        <v>320</v>
+      </c>
+      <c r="BG49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:60">
+      <c r="A50">
+        <v>55</v>
+      </c>
+      <c r="B50" t="s">
+        <v>331</v>
+      </c>
+      <c r="C50" t="s">
+        <v>332</v>
+      </c>
+      <c r="D50" t="s">
+        <v>333</v>
+      </c>
+      <c r="E50" t="s">
+        <v>334</v>
+      </c>
+      <c r="F50" t="s">
+        <v>334</v>
+      </c>
+      <c r="T50" t="s">
+        <v>335</v>
+      </c>
+      <c r="U50" t="s">
+        <v>336</v>
+      </c>
+      <c r="AQ50">
+        <v>200000</v>
+      </c>
+      <c r="AR50">
+        <v>250000</v>
+      </c>
+      <c r="AS50">
+        <v>2000000000</v>
+      </c>
+      <c r="AT50">
+        <v>30000</v>
+      </c>
+      <c r="AU50" t="s">
+        <v>326</v>
+      </c>
+      <c r="BG50">
+        <v>1</v>
+      </c>
+      <c r="BH50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:60">
+      <c r="A51">
+        <v>56</v>
+      </c>
+      <c r="B51" t="s">
+        <v>337</v>
+      </c>
+      <c r="C51" t="s">
+        <v>338</v>
+      </c>
+      <c r="D51" t="s">
+        <v>339</v>
+      </c>
+      <c r="E51" t="s">
+        <v>340</v>
+      </c>
+      <c r="F51" t="s">
+        <v>340</v>
+      </c>
+      <c r="T51" t="s">
+        <v>341</v>
+      </c>
+      <c r="AQ51">
+        <v>500000</v>
+      </c>
+      <c r="AR51">
+        <v>500000</v>
+      </c>
+      <c r="AS51">
+        <v>50000000000</v>
+      </c>
+      <c r="AT51">
+        <v>125000</v>
+      </c>
+      <c r="AU51" t="s">
+        <v>331</v>
+      </c>
+      <c r="BG51">
+        <v>2</v>
+      </c>
+      <c r="BH51">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>